<commit_message>
Scripting DPLKKPS001-010 and DPLKKPS001-011
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-010 - Kepesertaan - Setup Group Approval Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-010 - Kepesertaan - Setup Group Approval Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94AA754-8686-4C46-9801-45E151F35E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C61B8A-4EF3-4D6E-AB44-44124B8CB107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -49,12 +49,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>Putri</t>
-  </si>
-  <si>
-    <t>bni1234/</t>
-  </si>
-  <si>
     <t>MAIN_SIDEBAR</t>
   </si>
   <si>
@@ -109,30 +103,33 @@
     <t>Hapus Setup Group Approval</t>
   </si>
   <si>
-    <t>Username : Putri;
-Password : bni1234/;
+    <t>Setup Group Approval</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>bni1234</t>
+  </si>
+  <si>
+    <t>Username : 32382;
+Password : bni1234;
 Kode Group Approval : 9;
 Nama Group Approval : Editor</t>
   </si>
   <si>
-    <t>Username : Putri;
-Password : bni1234/;
+    <t>Username : 32382;
+Password : bni1234;
 Kode Group Approval : 9</t>
   </si>
   <si>
-    <t>Username : Putri;
-Password : bni1234/;
+    <t>Username : 32382;
+Password : bni1234;
 Kode Group Approval : 9;
 Nama Group Approval : Regulator</t>
-  </si>
-  <si>
-    <t>Setup Group Approval</t>
-  </si>
-  <si>
-    <t>Editor</t>
-  </si>
-  <si>
-    <t>Regulator</t>
   </si>
 </sst>
 </file>
@@ -525,7 +522,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -580,7 +577,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -589,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
@@ -603,43 +600,43 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M2" s="4">
         <v>9</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
@@ -655,37 +652,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M3" s="4">
         <v>9</v>
@@ -702,43 +699,43 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M4" s="4">
         <v>9</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="6"/>
@@ -752,37 +749,37 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M5" s="4">
         <v>9</v>

</xml_diff>